<commit_message>
unit + AI stats & AI
(COMPLETE)
</commit_message>
<xml_diff>
--- a/Mythos High/Assets/Stats/Character and Minion Stats.xlsx
+++ b/Mythos High/Assets/Stats/Character and Minion Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="169">
   <si>
     <t>Swordsman</t>
   </si>
@@ -96,30 +96,15 @@
     <t>Weapon Stats</t>
   </si>
   <si>
-    <t>Unit</t>
-  </si>
-  <si>
     <t>enemy w/in range</t>
   </si>
   <si>
     <t>enemy outside range</t>
   </si>
   <si>
-    <t>move along</t>
-  </si>
-  <si>
     <t>low health</t>
   </si>
   <si>
-    <t>go back to base</t>
-  </si>
-  <si>
-    <t>if hero is low hp</t>
-  </si>
-  <si>
-    <t>attack/use damage spell</t>
-  </si>
-  <si>
     <t>Movement Stats</t>
   </si>
   <si>
@@ -228,9 +213,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>AI</t>
-  </si>
-  <si>
     <t>Effect on Allies</t>
   </si>
   <si>
@@ -444,14 +426,110 @@
     <t>Summon a contraption in an area</t>
   </si>
   <si>
-    <t>Skill Trigger</t>
+    <t>AI Key</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Move along</t>
+  </si>
+  <si>
+    <t>Minion</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low health </t>
+  </si>
+  <si>
+    <t>Go back to base</t>
+  </si>
+  <si>
+    <t>follow key 1 or 2</t>
+  </si>
+  <si>
+    <t>low health hero while outside minion range</t>
+  </si>
+  <si>
+    <t>low health hero while inside minion range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  attack hero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  attack nearest minion</t>
+  </si>
+  <si>
+    <t>forever on</t>
+  </si>
+  <si>
+    <t>minion/hero on contact with enemy unit</t>
+  </si>
+  <si>
+    <t>low health for hero/last remaining minion</t>
+  </si>
+  <si>
+    <t>enemy units in groups of 3 or more || enemy hero life with health =&lt; skill damage</t>
+  </si>
+  <si>
+    <t>low health ally minions while in contact with enemy || enemy hero life with health =&lt; skill damage</t>
+  </si>
+  <si>
+    <t>enemy units in groups of 3 or more || fleeing low health hero</t>
+  </si>
+  <si>
+    <t>enemy units w/in attack range</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> enemy hero life with health =&lt; skill damage || fleeing hero w/out nearby ally units</t>
+  </si>
+  <si>
+    <t>enemy units w/in attack range when with ally minions or near base</t>
+  </si>
+  <si>
+    <t>when group of 3 or more ally minions are being attacked by 3 or more enemy units</t>
+  </si>
+  <si>
+    <t>enemy hero life with health =&lt; skill damage ||fleeing hero w/out nearby minions</t>
+  </si>
+  <si>
+    <t>low health without any nearby minions (4m)</t>
+  </si>
+  <si>
+    <t>whenever in contact with hero</t>
+  </si>
+  <si>
+    <t>Cooldown</t>
+  </si>
+  <si>
+    <t>13 sec</t>
+  </si>
+  <si>
+    <t>15 sec</t>
+  </si>
+  <si>
+    <t>17 sec</t>
+  </si>
+  <si>
+    <t>8 sec</t>
+  </si>
+  <si>
+    <t>12 sec</t>
+  </si>
+  <si>
+    <t>14 sec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,8 +591,28 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,6 +700,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -838,9 +954,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -973,6 +1086,99 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,32 +1491,32 @@
     <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="36" customFormat="1">
-      <c r="A1" s="36" t="s">
-        <v>53</v>
+    <row r="1" spans="1:16" s="35" customFormat="1">
+      <c r="A1" s="35" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1"/>
     <row r="3" spans="1:16" s="3" customFormat="1" ht="31.5" thickBot="1">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="23"/>
       <c r="F3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="23"/>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
       <c r="N3" s="24"/>
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
@@ -1590,36 +1796,36 @@
         <v>17</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N12" s="2"/>
     </row>
@@ -1663,41 +1869,41 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16" s="40" customFormat="1">
-      <c r="A14" s="37" t="s">
+    <row r="14" spans="1:16" s="39" customFormat="1">
+      <c r="A14" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="42">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="41">
         <v>0.3</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="41">
         <v>0.3</v>
       </c>
-      <c r="J14" s="42">
+      <c r="J14" s="41">
         <v>0.3</v>
       </c>
-      <c r="K14" s="42">
+      <c r="K14" s="41">
         <v>0.4</v>
       </c>
-      <c r="L14" s="41">
+      <c r="L14" s="40">
         <v>1</v>
       </c>
-      <c r="M14" s="42">
+      <c r="M14" s="41">
         <v>1</v>
       </c>
-      <c r="N14" s="38"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
     </row>
     <row r="15" spans="1:16" s="31" customFormat="1">
       <c r="A15" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1815,39 +2021,39 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="L19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="N19" s="12"/>
       <c r="O19" s="13"/>
@@ -1950,568 +2156,636 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="72.85546875" style="50" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="44" customWidth="1"/>
-    <col min="4" max="4" width="73" style="44" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" style="44" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" style="44" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" style="44" customWidth="1"/>
-    <col min="8" max="8" width="19" style="44" customWidth="1"/>
-    <col min="9" max="9" width="44" style="44" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="57.7109375" style="43" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" style="49" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="73" style="43" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" style="43" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" style="43" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" style="43" customWidth="1"/>
+    <col min="8" max="8" width="19" style="43" customWidth="1"/>
+    <col min="9" max="9" width="44" style="43" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="43" customFormat="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:8" s="42" customFormat="1">
+      <c r="A1" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="42" customFormat="1">
+      <c r="A3" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="50" customFormat="1">
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+    </row>
+    <row r="6" spans="1:8" s="44" customFormat="1">
+      <c r="A6" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="44" customFormat="1">
+      <c r="A8" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="50" customFormat="1">
+      <c r="A10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+    </row>
+    <row r="11" spans="1:8" s="45" customFormat="1">
+      <c r="A11" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="45" customFormat="1">
+      <c r="A13" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="50" customFormat="1">
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+    </row>
+    <row r="16" spans="1:8" s="46" customFormat="1">
+      <c r="A16" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="53" t="s">
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="46" customFormat="1">
+      <c r="A18" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="46" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="50" customFormat="1">
+      <c r="A20" s="72"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+    </row>
+    <row r="21" spans="1:8" s="50" customFormat="1">
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+    </row>
+    <row r="22" spans="1:8" s="47" customFormat="1">
+      <c r="A22" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="74"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="55" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="54" t="s">
+      <c r="F23" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="47" customFormat="1">
+      <c r="A24" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="50" customFormat="1">
+      <c r="A26" s="58"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+    </row>
+    <row r="27" spans="1:8" s="48" customFormat="1">
+      <c r="A27" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="78"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="43" customFormat="1">
-      <c r="A3" s="57" t="s">
+      <c r="E28" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="48" customFormat="1">
+      <c r="A29" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="79" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="53" t="s">
+      <c r="G29" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="54" t="s">
+      <c r="D30" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="51" customFormat="1">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-    </row>
-    <row r="6" spans="1:7" s="45" customFormat="1">
-      <c r="A6" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="45" customFormat="1">
-      <c r="A8" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="62" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="51" customFormat="1">
-      <c r="A10" s="59"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-    </row>
-    <row r="11" spans="1:7" s="46" customFormat="1">
-      <c r="A11" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="46" customFormat="1">
-      <c r="A13" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="G14" s="56" t="s">
+      <c r="G30" s="55" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="51" customFormat="1">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-    </row>
-    <row r="16" spans="1:7" s="47" customFormat="1">
-      <c r="A16" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="70"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="D17" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="47" customFormat="1">
-      <c r="A18" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="70" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="71" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="71" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="56" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="E19" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="51" customFormat="1">
-      <c r="A20" s="73"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-    </row>
-    <row r="21" spans="1:7" s="51" customFormat="1">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-    </row>
-    <row r="22" spans="1:7" s="48" customFormat="1">
-      <c r="A22" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="75"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="54" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" s="55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="48" customFormat="1">
-      <c r="A24" s="77" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="75" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="76" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="76" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="56" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="51" customFormat="1">
-      <c r="A26" s="59"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-    </row>
-    <row r="27" spans="1:7" s="49" customFormat="1">
-      <c r="A27" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="C28" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="49" customFormat="1">
-      <c r="A29" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="D29" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="80" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="80" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="54" t="s">
+      <c r="H30" s="43" t="s">
         <v>124</v>
-      </c>
-      <c r="B30" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="56" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B4 D1:XFD4">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C4">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2523,7 +2797,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C4">
+  <conditionalFormatting sqref="H17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2542,303 +2816,407 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="74.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51" style="81" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" style="97" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5">
-      <c r="A1" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="114" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="115" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="114" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="115" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="115" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="16.5">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="81">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5">
+      <c r="A3" s="105">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="106" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="106" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="107" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5">
+      <c r="A4" s="81">
+        <v>1.2</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5">
+      <c r="A5" s="105">
+        <v>2</v>
+      </c>
+      <c r="B5" s="107" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="D5" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="107" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5">
+      <c r="A6" s="81">
+        <v>3</v>
+      </c>
+      <c r="B6" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5">
+      <c r="A7" s="105">
+        <v>3.1</v>
+      </c>
+      <c r="B7" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.5">
-      <c r="A3" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="34" t="s">
+      <c r="D7" s="107"/>
+      <c r="E7" s="107" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17.25">
+      <c r="A8" s="101"/>
+      <c r="B8" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="104"/>
+    </row>
+    <row r="9" spans="1:5" ht="17.25">
+      <c r="A9" s="81">
+        <v>4</v>
+      </c>
+      <c r="B9" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="99" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25">
+      <c r="A10" s="81">
+        <v>5</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="108" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25">
+      <c r="A11" s="81">
+        <v>6</v>
+      </c>
+      <c r="B11" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="99" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25">
+      <c r="A12" s="101"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="102"/>
+    </row>
+    <row r="13" spans="1:5" ht="17.25">
+      <c r="A13" s="101"/>
+      <c r="B13" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="102"/>
+    </row>
+    <row r="14" spans="1:5" ht="17.25">
+      <c r="A14" s="81">
+        <v>7</v>
+      </c>
+      <c r="B14" s="84" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="99" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25">
+      <c r="A15" s="81">
+        <v>8</v>
+      </c>
+      <c r="B15" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="110" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17.25">
+      <c r="A16" s="81">
+        <v>9</v>
+      </c>
+      <c r="B16" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="99" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25">
+      <c r="A17" s="101"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="102"/>
+    </row>
+    <row r="18" spans="1:3" ht="17.25">
+      <c r="A18" s="101"/>
+      <c r="B18" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="102"/>
+    </row>
+    <row r="19" spans="1:3" ht="17.25">
+      <c r="A19" s="81">
+        <v>10</v>
+      </c>
+      <c r="B19" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="99" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.25">
+      <c r="A20" s="81">
+        <v>11</v>
+      </c>
+      <c r="B20" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="109" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17.25">
+      <c r="A21" s="81">
+        <v>12</v>
+      </c>
+      <c r="B21" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17.25">
+      <c r="A22" s="101"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="102"/>
+    </row>
+    <row r="23" spans="1:3" ht="17.25">
+      <c r="A23" s="101"/>
+      <c r="B23" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="102"/>
+    </row>
+    <row r="24" spans="1:3" ht="17.25">
+      <c r="A24" s="81">
         <v>13</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.5">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.5">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5">
-      <c r="A6" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17.25">
-      <c r="A8" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25">
-      <c r="A9" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25">
-      <c r="A10" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="58" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25">
-      <c r="A11" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="60"/>
-    </row>
-    <row r="13" spans="1:5" ht="17.25">
-      <c r="A13" s="61" t="s">
+      <c r="B24" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17.25">
+      <c r="A25" s="81">
+        <v>14</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="111" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17.25">
+      <c r="A26" s="81">
+        <v>15</v>
+      </c>
+      <c r="B26" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="99" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17.25">
+      <c r="A27" s="101"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="102"/>
+    </row>
+    <row r="28" spans="1:3" ht="17.25">
+      <c r="A28" s="101"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="102"/>
+    </row>
+    <row r="29" spans="1:3" ht="17.25">
+      <c r="A29" s="101"/>
+      <c r="B29" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="62"/>
-    </row>
-    <row r="14" spans="1:5" ht="17.25">
-      <c r="A14" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25">
-      <c r="A15" s="64" t="s">
+      <c r="C29" s="102"/>
+    </row>
+    <row r="30" spans="1:3" ht="17.25">
+      <c r="A30" s="81">
+        <v>16</v>
+      </c>
+      <c r="B30" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="100" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.25">
+      <c r="A31" s="81">
+        <v>17</v>
+      </c>
+      <c r="B31" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="112" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.25">
+      <c r="A32" s="81">
+        <v>18</v>
+      </c>
+      <c r="B32" s="84" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="100" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25">
+      <c r="A33" s="101"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="103"/>
+    </row>
+    <row r="34" spans="1:3" ht="17.25">
+      <c r="A34" s="101"/>
+      <c r="B34" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="62" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25">
-      <c r="A16" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="17.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="60"/>
-    </row>
-    <row r="18" spans="1:2" ht="17.25">
-      <c r="A18" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="66"/>
-    </row>
-    <row r="19" spans="1:2" ht="17.25">
-      <c r="A19" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="17.25">
-      <c r="A20" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="66" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="17.25">
-      <c r="A21" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="60"/>
-    </row>
-    <row r="23" spans="1:2" ht="17.25">
-      <c r="A23" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="70"/>
-    </row>
-    <row r="24" spans="1:2" ht="17.25">
-      <c r="A24" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17.25">
-      <c r="A25" s="72" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17.25">
-      <c r="A26" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="55" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="17.25">
-      <c r="A27" s="73"/>
-      <c r="B27" s="60"/>
-    </row>
-    <row r="28" spans="1:2" ht="17.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="60"/>
-    </row>
-    <row r="29" spans="1:2" ht="17.25">
-      <c r="A29" s="74" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="75"/>
-    </row>
-    <row r="30" spans="1:2" ht="17.25">
-      <c r="A30" s="54" t="s">
+      <c r="C34" s="103"/>
+    </row>
+    <row r="35" spans="1:3" ht="17.25">
+      <c r="A35" s="81">
+        <v>19</v>
+      </c>
+      <c r="B35" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="17.25">
-      <c r="A31" s="77" t="s">
+      <c r="C35" s="100" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17.25">
+      <c r="A36" s="81">
+        <v>20</v>
+      </c>
+      <c r="B36" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="B31" s="75" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="17.25">
-      <c r="A32" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="55" t="s">
+      <c r="C36" s="113" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17.25">
+      <c r="A37" s="81">
+        <v>21</v>
+      </c>
+      <c r="B37" s="84" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="17.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="60"/>
-    </row>
-    <row r="34" spans="1:2" ht="17.25">
-      <c r="A34" s="78" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="79"/>
-    </row>
-    <row r="35" spans="1:2" ht="17.25">
-      <c r="A35" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="55" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="17.25">
-      <c r="A36" s="81" t="s">
-        <v>122</v>
-      </c>
-      <c r="B36" s="79" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="17.25">
-      <c r="A37" s="54" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="55" t="s">
-        <v>125</v>
-      </c>
+      <c r="C37" s="100" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="81"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A8:B11">
+  <conditionalFormatting sqref="B8:B11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -2851,5 +3229,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>